<commit_message>
Actualizacion Matriz de asignaciones
</commit_message>
<xml_diff>
--- a/Documento de actividades del proyecto final.xlsx
+++ b/Documento de actividades del proyecto final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kwzz1\Desktop\móviles 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SystemFits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2577EF6F-12B3-4F7D-8F95-08B11E90222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B84984E-E91C-40F2-8310-03D37EEAD45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Método Kanban</t>
   </si>
@@ -62,55 +62,190 @@
     <t>A la espera</t>
   </si>
   <si>
-    <t>Creacion del proyecto y repositorio - Jason</t>
+    <t>Se cambio el Nombre de la aplicacion en el menu y se elimino el boton-Jason</t>
   </si>
   <si>
-    <t>Bottom Navigation Bar - Jason</t>
+    <t>Correciones en los botones-Jan Carlo</t>
   </si>
   <si>
-    <t>Vista Menú principal - Leoncio</t>
+    <t>Implementacion del editar funcional en todos los dias de la semana -Jan Jan Carlo</t>
   </si>
   <si>
-    <t>Vista Registro - Jason</t>
+    <t>Vista Medidas - Jan Carlo</t>
   </si>
   <si>
-    <t>Vista Login - Jason</t>
+    <t>Vista Alimentacion - Jan Carlo</t>
   </si>
   <si>
-    <t>Vista Ejercicio - Jason</t>
+    <t>Bottom Navigation Bar - Jason Esquivel</t>
   </si>
   <si>
-    <t>Vista Semana de ejercicios - Jason</t>
+    <t>Creacion del proyecto y repositorio - Jason Esquivel</t>
   </si>
   <si>
-    <t>Vista Ejercicios programados - Jason</t>
+    <t>Implementación de metodo editar y eliminar grupo muscular- Jan carlos</t>
   </si>
   <si>
-    <t>Vista Alimentacion - Jan</t>
+    <t>pop up para editar grupo muscular  - Jason Esquivel</t>
   </si>
   <si>
-    <t>Vista Medidas - Jan</t>
+    <t>Vista comida, diseño de calorias - Jan Carlos</t>
   </si>
   <si>
-    <t>Vista Recetas - Leoncio</t>
+    <t>Vista semana ejercicios funcionalidad crud  -Jan Carlos</t>
   </si>
   <si>
-    <t>Crear base de datos - Jason</t>
+    <t>Actualización y mejora de los fragment vista y menu- Jan carlos</t>
   </si>
   <si>
-    <t xml:space="preserve">Crear entidades para alimentacion y medidas - Jan </t>
+    <t>Vista Menu Principa - Jan Carlos</t>
   </si>
   <si>
-    <t>Crear entidades para login, registro y ejercicios - Jason</t>
+    <t>correciones -Jan Carlos</t>
   </si>
   <si>
-    <t>Crear api en php para las recetas - Leoncio</t>
+    <t>SystemFits App logo - Leoncio Pavon</t>
   </si>
   <si>
-    <t>Validar campos - Jan</t>
+    <t>Funciona editar y eliminar de la vista ejercicios - Jan Carlos Prado</t>
   </si>
   <si>
-    <t>Prueba</t>
+    <t>Readme- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Cambios en el nav_graph e implementacion de pop up editar ejercicio - Jan Carlos Prado</t>
+  </si>
+  <si>
+    <t>SystemFits Api pack - Leonico Pavon</t>
+  </si>
+  <si>
+    <t>Creacion Readme -Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Vista SemanaEjercicios validada e implementado el try catch - Jan Prado</t>
+  </si>
+  <si>
+    <t>Vista Ejercicios y configuracion validados y funcionales - Jan Carlos</t>
+  </si>
+  <si>
+    <t>Correccion de las SahredPref - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Correccion de los adapter a UI - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Correccion combo box Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Menu Principal funcional y correciones minimas- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Semana de Ejercicios funcionalidad y dias de la semana- Jason Esquivel</t>
+  </si>
+  <si>
+    <t>cambios en layout de recetas - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Funcionamiento del consumo de la API de recetas- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>permisos de internet - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Vista configuracion funcional, correcion de errores en login y registro - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>cambios en el fragment de recetas - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>cambios en el fragment del menu principal- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Implementación del DatePicker y Combo box de género en la Vista registro - Jan Prado</t>
+  </si>
+  <si>
+    <t>Update SystemFitBD.sql - Jan Prado</t>
+  </si>
+  <si>
+    <t>Vista registro - diseño, validacion y funcionalida, Vista login - Jan Prado</t>
+  </si>
+  <si>
+    <t>Nvarchar100 nombre ejercicio - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Modelo relacional de base de datos - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Cambios en los diseños de botones y pop up de agregar, editar y eliminar - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Error de login en backgorund resuelto - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Semana completa en editar Semana Ejercicios- Jason Esquivel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rediseño del LogIn - Leoncio Pavon
+navegacion a configuracion
+navegacion a configuracion
+navegacion a configuracion
+</t>
+  </si>
+  <si>
+    <t>Detalles Login - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>cambios minimos - Jan Prado</t>
+  </si>
+  <si>
+    <t>Creación de la vista de recetas- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>creacion de paquete vistas- Jan Prado</t>
+  </si>
+  <si>
+    <t>Campos de comida y medidas validos y correciones minimas en los item - Jan Prado</t>
+  </si>
+  <si>
+    <t>entidad comida, comidaDao, comidaAdapter, comidasViewModel, crud areglos minimos en los item de comida y medida- Jan Prado</t>
+  </si>
+  <si>
+    <t>Entidad medida, medidasDao, medidasAdapter, medidasViewModel, Crud - Jan Prado</t>
+  </si>
+  <si>
+    <t>Creación de la vista items del RCV del Menu principal - Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Creación de la vista del Menu principal- Leoncio Pavon</t>
+  </si>
+  <si>
+    <t>Semana ya tiene una pestania propia y un popup para agregar datos -Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Documentos Requeridos - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Dia De la semamana se marca en RB y EN tv de fragment ejercicios
+Dia De la semamana se marca en RB y EN tv de fragment ejercicios
+Dia De la semamana se marca en RB y EN tv de fragment ejercicios
+Dia De la semamana se marca en RB y EN tv de fragment ejercicios
+Dia De la semamana se marca en RB y EN tv de fragment ejercicios
+Dia De la semamana se marca en RB y EN tv de fragment ejercicios - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Se agrego el disenio de ejercicios y la edicion de ejercicios - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Vista alimentacion, agregar comida, editar comida, Vista medidas -Jan Prado</t>
+  </si>
+  <si>
+    <t>Cosas con version antigua (Funcionalidades) - Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Initial commit, footmenu funcional y ocultable -Jason Esquivel</t>
+  </si>
+  <si>
+    <t>Actualizacion Matriz de asignaciones - Jason esquivel</t>
   </si>
 </sst>
 </file>
@@ -162,17 +297,6 @@
       <name val="Source Sans Pro"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Source Sans Pro"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color rgb="FF17365D"/>
-      <name val="Source Sans Pro"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color rgb="FF17365D"/>
@@ -180,18 +304,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Source Sans Pro"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Source Sans Pro"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <color theme="1"/>
       <name val="Source Sans Pro"/>
     </font>
@@ -207,8 +320,35 @@
       <name val="Source Sans Pro"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF17365D"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
@@ -427,7 +567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,59 +582,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,7 +600,67 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -731,7 +888,7 @@
     <col min="2" max="2" width="79.375" customWidth="1"/>
     <col min="3" max="3" width="60.75" customWidth="1"/>
     <col min="4" max="4" width="62.25" customWidth="1"/>
-    <col min="5" max="5" width="67.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="112.125" customWidth="1"/>
     <col min="6" max="6" width="36.875" customWidth="1"/>
     <col min="7" max="26" width="10" customWidth="1"/>
   </cols>
@@ -766,12 +923,12 @@
     </row>
     <row r="2" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -796,14 +953,14 @@
     </row>
     <row r="3" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="1"/>
@@ -830,14 +987,14 @@
     </row>
     <row r="4" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="31"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="5"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -860,19 +1017,15 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="20" t="s">
-        <v>17</v>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="34" t="s">
+        <v>12</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -894,21 +1047,15 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="20" t="s">
-        <v>18</v>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="35" t="s">
+        <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -930,21 +1077,15 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="20" t="s">
-        <v>19</v>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="36" t="s">
+        <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -966,19 +1107,15 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="20" t="s">
-        <v>20</v>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="36" t="s">
+        <v>9</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1000,17 +1137,15 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="35" t="s">
-        <v>22</v>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="32" t="s">
+        <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1032,15 +1167,15 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="20" t="s">
-        <v>21</v>
+      <c r="B10" s="19"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="32" t="s">
+        <v>8</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1062,13 +1197,15 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1090,13 +1227,15 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1118,13 +1257,15 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1146,13 +1287,15 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1174,13 +1317,15 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1202,13 +1347,15 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="8"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1230,12 +1377,14 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1258,12 +1407,14 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="32" t="s">
+        <v>19</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1286,12 +1437,14 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="37" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1314,12 +1467,14 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="32" t="s">
+        <v>21</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1342,12 +1497,14 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="32" t="s">
+        <v>22</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1370,12 +1527,14 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="33" t="s">
+        <v>23</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1398,13 +1557,15 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="10"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1426,12 +1587,14 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="32" t="s">
+        <v>25</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1454,12 +1617,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="32" t="s">
+        <v>26</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1482,13 +1647,15 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="21"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="10"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1510,12 +1677,14 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1538,12 +1707,14 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="32" t="s">
+        <v>29</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1566,13 +1737,15 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="21"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="10"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1594,12 +1767,14 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="32" t="s">
+        <v>31</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -1622,12 +1797,14 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1650,13 +1827,15 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="10"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1678,12 +1857,14 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="32" t="s">
+        <v>34</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -1706,12 +1887,14 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -1734,13 +1917,15 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="21"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="10"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1762,12 +1947,14 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="32" t="s">
+        <v>37</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -1790,12 +1977,14 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="32" t="s">
+        <v>38</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -1818,12 +2007,14 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="32" t="s">
+        <v>39</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -1846,13 +2037,15 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="21"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="10"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -1874,12 +2067,14 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="33" t="s">
+        <v>41</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -1902,12 +2097,14 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="24"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="39" t="s">
+        <v>42</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -1930,12 +2127,14 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="24"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="33" t="s">
+        <v>43</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -1958,12 +2157,14 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="24"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -1986,12 +2187,14 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="24"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="39" t="s">
+        <v>45</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2014,12 +2217,14 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="24"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2042,12 +2247,14 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="24"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="40" t="s">
+        <v>47</v>
+      </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -2070,12 +2277,14 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="24"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2098,12 +2307,14 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="24"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="39" t="s">
+        <v>49</v>
+      </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2126,12 +2337,14 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="24"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="39" t="s">
+        <v>50</v>
+      </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -2154,12 +2367,14 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="24"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="39" t="s">
+        <v>51</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2182,12 +2397,14 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="24"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2210,12 +2427,14 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="24"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="39" t="s">
+        <v>53</v>
+      </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2238,12 +2457,14 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="24"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="33" t="s">
+        <v>54</v>
+      </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2266,12 +2487,14 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="24"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2294,12 +2517,14 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="24"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="39" t="s">
+        <v>56</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2322,12 +2547,14 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="24"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="39" t="s">
+        <v>57</v>
+      </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -2350,12 +2577,14 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="23"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="24"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="39" t="s">
+        <v>58</v>
+      </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -2378,12 +2607,14 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="24"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="40" t="s">
+        <v>59</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -2406,12 +2637,14 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="23"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="24"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="39" t="s">
+        <v>60</v>
+      </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -2434,12 +2667,14 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="24"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="39" t="s">
+        <v>61</v>
+      </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -2462,12 +2697,14 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="24"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="39" t="s">
+        <v>62</v>
+      </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -2490,12 +2727,14 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="23"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="24"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="39" t="s">
+        <v>63</v>
+      </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -2518,12 +2757,14 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="23"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="24"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -2546,12 +2787,12 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="24"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="28"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -2574,12 +2815,12 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="23"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="24"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="28"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -2602,12 +2843,12 @@
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
     </row>
-    <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="23"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="24"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="28"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -2630,12 +2871,12 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="27"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="31"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>

</xml_diff>